<commit_message>
Starting diversity indices analysis
</commit_message>
<xml_diff>
--- a/Stats_Results.xlsx
+++ b/Stats_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SSD_1Tb_PF/Work/torrey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCBD61B-9347-EE43-9606-B1C521035C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C442B64E-1FF0-B344-98D6-B774EA1EA840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{427BFFD6-8046-594F-BD1A-82F8D9FA486D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{427BFFD6-8046-594F-BD1A-82F8D9FA486D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="107">
   <si>
     <t>Df</t>
   </si>
@@ -285,13 +285,85 @@
   </si>
   <si>
     <t>Permdisp NS</t>
+  </si>
+  <si>
+    <t>group1</t>
+  </si>
+  <si>
+    <t>&lt;chr&gt;</t>
+  </si>
+  <si>
+    <t>group2</t>
+  </si>
+  <si>
+    <t>&lt;dbl&gt;</t>
+  </si>
+  <si>
+    <t>F_value</t>
+  </si>
+  <si>
+    <t>df1</t>
+  </si>
+  <si>
+    <t>df2</t>
+  </si>
+  <si>
+    <t>p_value</t>
+  </si>
+  <si>
+    <t>Bivalve beds</t>
+  </si>
+  <si>
+    <t>FPS</t>
+  </si>
+  <si>
+    <t>0.178</t>
+  </si>
+  <si>
+    <t>0.111</t>
+  </si>
+  <si>
+    <t>Impacted</t>
+  </si>
+  <si>
+    <t>0.202</t>
+  </si>
+  <si>
+    <t>0.017</t>
+  </si>
+  <si>
+    <t>0.184</t>
+  </si>
+  <si>
+    <t>0.125</t>
+  </si>
+  <si>
+    <t>Pairwise function</t>
+  </si>
+  <si>
+    <t>0.256</t>
+  </si>
+  <si>
+    <t>0.038</t>
+  </si>
+  <si>
+    <t>0.239</t>
+  </si>
+  <si>
+    <t>0.012</t>
+  </si>
+  <si>
+    <t>0.266</t>
+  </si>
+  <si>
+    <t>0.041</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -349,6 +421,25 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="DejaVu Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Lucida Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Lucida Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -431,7 +522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -452,6 +543,14 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -459,15 +558,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EA06066-730F-AC47-8C37-A79A1AD98C17}">
-  <dimension ref="A1:AF69"/>
+  <dimension ref="A1:AF79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="U47" sqref="U47"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="137" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -815,44 +911,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="25" customHeight="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="J1" s="21" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="J1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="Y1" s="21" t="s">
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="Y1" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="23"/>
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="23"/>
+      <c r="AF1" s="23"/>
     </row>
     <row r="2" spans="1:32" ht="20">
-      <c r="A2" s="18"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
       <c r="J2" s="6" t="s">
         <v>12</v>
       </c>
@@ -969,7 +1065,6 @@
       </c>
       <c r="J6" s="6"/>
       <c r="X6" s="6"/>
-      <c r="Y6" s="23"/>
     </row>
     <row r="7" spans="1:32" ht="20">
       <c r="J7" s="6"/>
@@ -977,7 +1072,7 @@
       <c r="Y7" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="AB7" s="25"/>
+      <c r="AB7" s="20"/>
     </row>
     <row r="8" spans="1:32" ht="20">
       <c r="A8" s="6" t="s">
@@ -989,7 +1084,7 @@
       <c r="Y8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="AB8" s="25"/>
+      <c r="AB8" s="20"/>
       <c r="AC8" t="s">
         <v>78</v>
       </c>
@@ -1010,6 +1105,9 @@
       <c r="X10" s="6"/>
     </row>
     <row r="11" spans="1:32" ht="20">
+      <c r="A11" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="J11" s="6" t="s">
         <v>35</v>
       </c>
@@ -1022,6 +1120,27 @@
       </c>
     </row>
     <row r="12" spans="1:32" ht="20">
+      <c r="A12" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>90</v>
+      </c>
       <c r="J12" s="6" t="s">
         <v>36</v>
       </c>
@@ -1030,6 +1149,27 @@
       <c r="P12" s="10"/>
     </row>
     <row r="13" spans="1:32" ht="20">
+      <c r="A13" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>86</v>
+      </c>
       <c r="J13" s="6" t="s">
         <v>37</v>
       </c>
@@ -1037,740 +1177,957 @@
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
     </row>
-    <row r="15" spans="1:32" ht="22">
-      <c r="J15" s="21" t="s">
+    <row r="14" spans="1:32" ht="20">
+      <c r="A14" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="30">
+        <v>2411</v>
+      </c>
+      <c r="E14" s="29">
+        <v>1</v>
+      </c>
+      <c r="F14" s="29">
+        <v>7</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="J14" s="6"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+    </row>
+    <row r="15" spans="1:32" ht="20">
+      <c r="A15" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="30">
+        <v>3145</v>
+      </c>
+      <c r="E15" s="29">
+        <v>1</v>
+      </c>
+      <c r="F15" s="29">
+        <v>10</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="J15" s="6"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+    </row>
+    <row r="16" spans="1:32" ht="20">
+      <c r="A16" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="30">
+        <v>2531</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="29">
+        <v>7</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="J16" s="6"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+    </row>
+    <row r="17" spans="1:32" ht="20">
+      <c r="J17" s="6"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+    </row>
+    <row r="19" spans="1:32" ht="22">
+      <c r="J19" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="Y15" s="21" t="s">
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="Y19" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="Z15" s="21"/>
-      <c r="AA15" s="21"/>
-      <c r="AB15" s="21"/>
-      <c r="AC15" s="21"/>
-      <c r="AD15" s="21"/>
-      <c r="AE15" s="21"/>
-      <c r="AF15" s="21"/>
-    </row>
-    <row r="16" spans="1:32" ht="20">
-      <c r="A16" s="18" t="s">
+      <c r="Z19" s="23"/>
+      <c r="AA19" s="23"/>
+      <c r="AB19" s="23"/>
+      <c r="AC19" s="23"/>
+      <c r="AD19" s="23"/>
+      <c r="AE19" s="23"/>
+      <c r="AF19" s="23"/>
+    </row>
+    <row r="20" spans="1:32" ht="20">
+      <c r="A20" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B20" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="J16" s="6" t="s">
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="J20" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:30" ht="20">
-      <c r="A17" s="18"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="J17" s="6" t="s">
+    <row r="21" spans="1:32" ht="20">
+      <c r="A21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="J21" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:30" ht="20">
-      <c r="B18" s="20" t="s">
+    <row r="22" spans="1:32" ht="20">
+      <c r="B22" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C22" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D22" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E22" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="J18" s="6" t="s">
+      <c r="J22" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="R18" t="s">
+      <c r="R22" t="s">
         <v>49</v>
       </c>
-      <c r="Y18" s="6" t="s">
+      <c r="Y22" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:30" ht="20">
-      <c r="A19" s="12" t="s">
+    <row r="23" spans="1:32" ht="20">
+      <c r="A23" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="J19" s="6" t="s">
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="J23" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="Y19" s="6" t="s">
+      <c r="Y23" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:30" ht="20">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="Y20" s="6" t="s">
+    <row r="24" spans="1:32" ht="20">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="Y24" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:30" ht="20">
-      <c r="A21" s="3" t="s">
+    <row r="25" spans="1:32" ht="20">
+      <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B25" s="3">
         <v>4</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C25" s="3">
         <v>0.74587349999999997</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D25" s="3">
         <v>0.640791</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E25" s="3">
         <v>4.4597360000000004</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F25" s="13">
         <v>1E-3</v>
       </c>
-      <c r="G21" s="24" t="s">
+      <c r="G25" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="J21" s="6" t="s">
+      <c r="J25" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="Y21" s="23"/>
-    </row>
-    <row r="22" spans="1:30" ht="20">
-      <c r="A22" s="3" t="s">
+    </row>
+    <row r="26" spans="1:32" ht="20">
+      <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B26" s="3">
         <v>10</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C26" s="3">
         <v>0.41811530000000002</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D26" s="3">
         <v>0.359209</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J22" s="6" t="s">
+      <c r="J26" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Y22" s="6" t="s">
+      <c r="Y26" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AB22" s="25"/>
-      <c r="AD22" t="s">
+      <c r="AB26" s="20"/>
+      <c r="AD26" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:30" ht="20">
-      <c r="A23" s="3" t="s">
+    <row r="27" spans="1:32" ht="20">
+      <c r="A27" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B27" s="3">
         <v>14</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C27" s="3">
         <v>1.1639887</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D27" s="3">
         <v>1</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J23" s="6" t="s">
+      <c r="J27" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y23" s="6" t="s">
+      <c r="Y27" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="AB23" s="25"/>
-    </row>
-    <row r="24" spans="1:30" ht="20">
-      <c r="J24" s="6" t="s">
+      <c r="AB27" s="20"/>
+    </row>
+    <row r="28" spans="1:32" ht="20">
+      <c r="J28" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-    </row>
-    <row r="25" spans="1:30" ht="20">
-      <c r="J25" s="6" t="s">
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+    </row>
+    <row r="29" spans="1:32" ht="20">
+      <c r="J29" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="K25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="R25" t="s">
+      <c r="K29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="R29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:30" ht="20">
-      <c r="J26" s="6" t="s">
+    <row r="30" spans="1:32" ht="20">
+      <c r="J30" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="K26" s="10"/>
-      <c r="O26" s="10"/>
-    </row>
-    <row r="27" spans="1:30" ht="20">
-      <c r="J27" s="6" t="s">
+      <c r="K30" s="10"/>
+      <c r="O30" s="10"/>
+    </row>
+    <row r="31" spans="1:32" ht="20">
+      <c r="J31" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-    </row>
-    <row r="28" spans="1:30" ht="20">
-      <c r="J28" s="6" t="s">
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+    </row>
+    <row r="32" spans="1:32" ht="20">
+      <c r="J32" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K28" s="10"/>
-    </row>
-    <row r="31" spans="1:30" s="14" customFormat="1"/>
-    <row r="32" spans="1:30" s="14" customFormat="1"/>
-    <row r="33" spans="1:29" s="14" customFormat="1"/>
-    <row r="39" spans="1:29" ht="22">
-      <c r="A39" s="18" t="s">
+      <c r="K32" s="10"/>
+    </row>
+    <row r="35" spans="1:29" s="14" customFormat="1"/>
+    <row r="36" spans="1:29" s="14" customFormat="1"/>
+    <row r="37" spans="1:29" s="14" customFormat="1"/>
+    <row r="43" spans="1:29" ht="22">
+      <c r="A43" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B43" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="5"/>
-      <c r="J39" s="21" t="s">
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="5"/>
+      <c r="J43" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="K39" s="21"/>
-      <c r="L39" s="21"/>
-      <c r="M39" s="21"/>
-      <c r="N39" s="21"/>
-      <c r="O39" s="21"/>
-      <c r="P39" s="21"/>
-      <c r="Q39" s="21"/>
-      <c r="V39" s="21" t="s">
+      <c r="K43" s="23"/>
+      <c r="L43" s="23"/>
+      <c r="M43" s="23"/>
+      <c r="N43" s="23"/>
+      <c r="O43" s="23"/>
+      <c r="P43" s="23"/>
+      <c r="Q43" s="23"/>
+      <c r="V43" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="W39" s="21"/>
-      <c r="X39" s="21"/>
-      <c r="Y39" s="21"/>
-      <c r="Z39" s="21"/>
-      <c r="AA39" s="21"/>
-      <c r="AB39" s="21"/>
-      <c r="AC39" s="21"/>
-    </row>
-    <row r="40" spans="1:29" ht="22">
-      <c r="A40" s="18"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="5"/>
-      <c r="J40" s="6" t="s">
+      <c r="W43" s="23"/>
+      <c r="X43" s="23"/>
+      <c r="Y43" s="23"/>
+      <c r="Z43" s="23"/>
+      <c r="AA43" s="23"/>
+      <c r="AB43" s="23"/>
+      <c r="AC43" s="23"/>
+    </row>
+    <row r="44" spans="1:29" ht="22">
+      <c r="A44" s="24"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="5"/>
+      <c r="J44" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K40" s="7"/>
-      <c r="L40" s="7"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="7"/>
-    </row>
-    <row r="41" spans="1:29" ht="22">
-      <c r="B41" s="20" t="s">
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+    </row>
+    <row r="45" spans="1:29" ht="22">
+      <c r="B45" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C45" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="20" t="s">
+      <c r="D45" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="E45" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="J41" s="6" t="s">
+      <c r="J45" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
-      <c r="N41" s="7"/>
-      <c r="O41" s="7"/>
-      <c r="V41" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:29" ht="22">
-      <c r="A42" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="G42" s="1"/>
-      <c r="J42" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="15"/>
-      <c r="P42" s="16"/>
-      <c r="Q42" s="16"/>
-      <c r="V42" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="1:29" ht="22">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="J43" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="7"/>
-      <c r="N43" s="7"/>
-      <c r="O43" s="7"/>
-      <c r="V43" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="44" spans="1:29" ht="22">
-      <c r="A44" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B44" s="3">
-        <v>2</v>
-      </c>
-      <c r="C44" s="3">
-        <v>0.56172060000000001</v>
-      </c>
-      <c r="D44" s="3">
-        <v>0.24625540000000001</v>
-      </c>
-      <c r="E44" s="3">
-        <v>1.960256</v>
-      </c>
-      <c r="F44" s="9">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G44" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="H44" s="16"/>
-      <c r="J44" s="7"/>
-      <c r="V44" s="23"/>
-    </row>
-    <row r="45" spans="1:29" ht="22">
-      <c r="A45" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" s="3">
-        <v>12</v>
-      </c>
-      <c r="C45" s="3">
-        <v>1.7193286000000001</v>
-      </c>
-      <c r="D45" s="3">
-        <v>0.75374459999999999</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G45" t="s">
-        <v>56</v>
-      </c>
-      <c r="J45" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="K45" s="7"/>
       <c r="L45" s="7"/>
       <c r="M45" s="7"/>
       <c r="N45" s="7"/>
       <c r="O45" s="7"/>
-      <c r="P45" s="7"/>
       <c r="V45" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" ht="22">
+      <c r="A46" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="G46" s="1"/>
+      <c r="J46" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="16"/>
+      <c r="Q46" s="16"/>
+      <c r="V46" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" ht="22">
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="J47" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
+      <c r="V47" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29" ht="22">
+      <c r="A48" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="3">
+        <v>2</v>
+      </c>
+      <c r="C48" s="3">
+        <v>0.56172060000000001</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0.24625540000000001</v>
+      </c>
+      <c r="E48" s="3">
+        <v>1.960256</v>
+      </c>
+      <c r="F48" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G48" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H48" s="16"/>
+      <c r="J48" s="7"/>
+    </row>
+    <row r="49" spans="1:29" ht="22">
+      <c r="A49" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="3">
+        <v>12</v>
+      </c>
+      <c r="C49" s="3">
+        <v>1.7193286000000001</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0.75374459999999999</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="7"/>
+      <c r="P49" s="7"/>
+      <c r="V49" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="Y45" s="26"/>
-      <c r="AA45" t="s">
+      <c r="Y49" s="21"/>
+      <c r="AA49" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:29" ht="20">
-      <c r="A46" s="3" t="s">
+    <row r="50" spans="1:29" ht="20">
+      <c r="A50" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B50" s="3">
         <v>14</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C50" s="3">
         <v>2.2810492</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D50" s="3">
         <v>1</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E50" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="F50" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J46" s="6" t="s">
+      <c r="J50" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="V46" s="6" t="s">
+      <c r="V50" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="Y46" s="25"/>
-    </row>
-    <row r="47" spans="1:29" ht="20">
-      <c r="J47" s="6" t="s">
+      <c r="Y50" s="20"/>
+    </row>
+    <row r="51" spans="1:29" ht="20">
+      <c r="J51" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="V47" s="23"/>
-    </row>
-    <row r="48" spans="1:29" ht="20">
-      <c r="A48" s="6" t="s">
+    </row>
+    <row r="52" spans="1:29" ht="20">
+      <c r="A52" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="J48" s="6" t="s">
+      <c r="J52" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="V48" s="6" t="s">
+      <c r="V52" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:29" ht="20">
-      <c r="A49" s="6" t="s">
+    <row r="53" spans="1:29" ht="20">
+      <c r="A53" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="J49" s="6" t="s">
+      <c r="J53" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="O49" s="10"/>
-      <c r="P49" s="10"/>
-      <c r="V49" s="6" t="s">
+      <c r="O53" s="10"/>
+      <c r="P53" s="10"/>
+      <c r="V53" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:29" ht="20">
-      <c r="J50" s="6" t="s">
+    <row r="54" spans="1:29" ht="20">
+      <c r="J54" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="M50" s="10"/>
-      <c r="N50" s="10"/>
-    </row>
-    <row r="51" spans="1:29" ht="20">
-      <c r="J51" s="6"/>
-    </row>
-    <row r="52" spans="1:29" ht="20">
-      <c r="J52" s="6"/>
-    </row>
-    <row r="53" spans="1:29" ht="22">
-      <c r="A53" s="18" t="s">
+      <c r="M54" s="10"/>
+      <c r="N54" s="10"/>
+    </row>
+    <row r="55" spans="1:29">
+      <c r="A55" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29" ht="20">
+      <c r="A56" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D56" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="E56" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="F56" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G56" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="J56" s="6"/>
+      <c r="M56" s="10"/>
+      <c r="N56" s="10"/>
+    </row>
+    <row r="57" spans="1:29" ht="20">
+      <c r="A57" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C57" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D57" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E57" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="F57" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G57" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="J57" s="6"/>
+      <c r="M57" s="10"/>
+      <c r="N57" s="10"/>
+    </row>
+    <row r="58" spans="1:29" ht="20">
+      <c r="A58" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B58" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C58" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D58" s="30">
+        <v>1519</v>
+      </c>
+      <c r="E58" s="29">
+        <v>1</v>
+      </c>
+      <c r="F58" s="29">
+        <v>7</v>
+      </c>
+      <c r="G58" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="J58" s="6"/>
+      <c r="M58" s="10"/>
+      <c r="N58" s="10"/>
+    </row>
+    <row r="59" spans="1:29" ht="20">
+      <c r="A59" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B59" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="D59" s="30">
+        <v>2526</v>
+      </c>
+      <c r="E59" s="29">
+        <v>1</v>
+      </c>
+      <c r="F59" s="29">
+        <v>10</v>
+      </c>
+      <c r="G59" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="J59" s="6"/>
+      <c r="M59" s="10"/>
+      <c r="N59" s="10"/>
+    </row>
+    <row r="60" spans="1:29" ht="20">
+      <c r="A60" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B60" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C60" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D60" s="30">
+        <v>1576</v>
+      </c>
+      <c r="E60" s="29">
+        <v>1</v>
+      </c>
+      <c r="F60" s="29">
+        <v>7</v>
+      </c>
+      <c r="G60" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="J60" s="6"/>
+      <c r="M60" s="10"/>
+      <c r="N60" s="10"/>
+    </row>
+    <row r="61" spans="1:29" ht="20">
+      <c r="J61" s="6"/>
+    </row>
+    <row r="62" spans="1:29" ht="20">
+      <c r="J62" s="6"/>
+    </row>
+    <row r="63" spans="1:29" ht="22">
+      <c r="A63" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="19" t="s">
+      <c r="B63" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="J53" s="21" t="s">
+      <c r="C63" s="25"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="25"/>
+      <c r="F63" s="25"/>
+      <c r="J63" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="K53" s="21"/>
-      <c r="L53" s="21"/>
-      <c r="M53" s="21"/>
-      <c r="N53" s="21"/>
-      <c r="O53" s="21"/>
-      <c r="P53" s="21"/>
-      <c r="Q53" s="21"/>
-      <c r="V53" s="21" t="s">
+      <c r="K63" s="23"/>
+      <c r="L63" s="23"/>
+      <c r="M63" s="23"/>
+      <c r="N63" s="23"/>
+      <c r="O63" s="23"/>
+      <c r="P63" s="23"/>
+      <c r="Q63" s="23"/>
+      <c r="V63" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="W53" s="21"/>
-      <c r="X53" s="21"/>
-      <c r="Y53" s="21"/>
-      <c r="Z53" s="21"/>
-      <c r="AA53" s="21"/>
-      <c r="AB53" s="21"/>
-      <c r="AC53" s="21"/>
-    </row>
-    <row r="54" spans="1:29">
-      <c r="A54" s="18"/>
-      <c r="B54" s="19"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19"/>
-    </row>
-    <row r="55" spans="1:29" ht="20">
-      <c r="J55" s="6" t="s">
+      <c r="W63" s="23"/>
+      <c r="X63" s="23"/>
+      <c r="Y63" s="23"/>
+      <c r="Z63" s="23"/>
+      <c r="AA63" s="23"/>
+      <c r="AB63" s="23"/>
+      <c r="AC63" s="23"/>
+    </row>
+    <row r="64" spans="1:29">
+      <c r="A64" s="24"/>
+      <c r="B64" s="25"/>
+      <c r="C64" s="25"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="25"/>
+      <c r="F64" s="25"/>
+    </row>
+    <row r="65" spans="1:27" ht="20">
+      <c r="J65" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:29" ht="20">
-      <c r="B56" s="20" t="s">
+    <row r="66" spans="1:27" ht="20">
+      <c r="B66" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C56" s="20" t="s">
+      <c r="C66" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D56" s="20" t="s">
+      <c r="D66" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E56" s="20" t="s">
+      <c r="E66" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="J56" s="6" t="s">
+      <c r="J66" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="V56" s="6" t="s">
+      <c r="V66" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:29" ht="20">
-      <c r="A57" s="12" t="s">
+    <row r="67" spans="1:27" ht="20">
+      <c r="A67" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
-      <c r="J57" s="6" t="s">
+      <c r="B67" s="26"/>
+      <c r="C67" s="26"/>
+      <c r="D67" s="26"/>
+      <c r="E67" s="26"/>
+      <c r="J67" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="P57" s="10"/>
-      <c r="Q57" s="10"/>
-      <c r="R57" s="10"/>
-      <c r="V57" s="6" t="s">
+      <c r="P67" s="10"/>
+      <c r="Q67" s="10"/>
+      <c r="R67" s="10"/>
+      <c r="V67" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:29" ht="20">
-      <c r="A58" s="12"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
-      <c r="J58" s="6" t="s">
+    <row r="68" spans="1:27" ht="20">
+      <c r="A68" s="12"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="J68" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="V58" s="6" t="s">
+      <c r="V68" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:29" ht="20">
-      <c r="A59" s="3" t="s">
+    <row r="69" spans="1:27" ht="20">
+      <c r="A69" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B69" s="3">
         <v>4</v>
       </c>
-      <c r="C59" s="3">
+      <c r="C69" s="3">
         <v>1.3009185999999999</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D69" s="3">
         <v>0.57031589999999999</v>
       </c>
-      <c r="E59" s="3">
+      <c r="E69" s="3">
         <v>3.318228</v>
       </c>
-      <c r="F59" s="22">
+      <c r="F69" s="18">
         <v>1E-3</v>
       </c>
-      <c r="G59" s="17" t="s">
+      <c r="G69" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="J59" s="6" t="s">
+      <c r="J69" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="V59" s="23"/>
-    </row>
-    <row r="60" spans="1:29" ht="20">
-      <c r="A60" s="3" t="s">
+    </row>
+    <row r="70" spans="1:27" ht="20">
+      <c r="A70" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B60" s="3">
+      <c r="B70" s="3">
         <v>10</v>
       </c>
-      <c r="C60" s="3">
+      <c r="C70" s="3">
         <v>0.98013059999999996</v>
       </c>
-      <c r="D60" s="3">
+      <c r="D70" s="3">
         <v>0.42968410000000001</v>
       </c>
-      <c r="E60" s="4" t="s">
+      <c r="E70" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F60" s="4" t="s">
+      <c r="F70" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J60" s="6" t="s">
+      <c r="J70" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="V60" s="6" t="s">
+      <c r="V70" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="Y60" s="27"/>
-    </row>
-    <row r="61" spans="1:29" ht="20">
-      <c r="A61" s="3" t="s">
+      <c r="Y70" s="22"/>
+    </row>
+    <row r="71" spans="1:27" ht="20">
+      <c r="A71" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B61" s="3">
+      <c r="B71" s="3">
         <v>14</v>
       </c>
-      <c r="C61" s="3">
+      <c r="C71" s="3">
         <v>2.2810492</v>
       </c>
-      <c r="D61" s="3">
+      <c r="D71" s="3">
         <v>1</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="E71" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F61" s="4" t="s">
+      <c r="F71" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="V61" s="6" t="s">
+      <c r="V71" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="Y61" s="25"/>
-      <c r="AA61" t="s">
+      <c r="Y71" s="20"/>
+      <c r="AA71" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="62" spans="1:29" ht="20">
-      <c r="J62" s="6" t="s">
+    <row r="72" spans="1:27" ht="20">
+      <c r="J72" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="V62" s="23"/>
-      <c r="AA62" t="s">
+      <c r="AA72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="1:29" ht="20">
-      <c r="J63" s="6" t="s">
+    <row r="73" spans="1:27" ht="20">
+      <c r="J73" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="V63" s="6" t="s">
+      <c r="V73" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="1:29" ht="20">
-      <c r="J64" s="6" t="s">
+    <row r="74" spans="1:27" ht="20">
+      <c r="J74" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="V64" s="6" t="s">
+      <c r="V74" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="10:15" ht="20">
-      <c r="J65" s="6" t="s">
+    <row r="75" spans="1:27" ht="20">
+      <c r="J75" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="66" spans="10:15" ht="20">
-      <c r="J66" s="6" t="s">
+    <row r="76" spans="1:27" ht="20">
+      <c r="J76" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="10:15" ht="20">
-      <c r="J67" s="6" t="s">
+    <row r="77" spans="1:27" ht="20">
+      <c r="J77" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="68" spans="10:15" ht="20">
-      <c r="J68" s="6" t="s">
+    <row r="78" spans="1:27" ht="20">
+      <c r="J78" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="69" spans="10:15" ht="20">
-      <c r="J69" s="6" t="s">
+    <row r="79" spans="1:27" ht="20">
+      <c r="J79" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="O69" s="10"/>
+      <c r="O79" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="V39:AC39"/>
-    <mergeCell ref="V53:AC53"/>
-    <mergeCell ref="J53:Q53"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:F64"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:F44"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="J43:Q43"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:F21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="J19:Q19"/>
+    <mergeCell ref="V43:AC43"/>
+    <mergeCell ref="V63:AC63"/>
+    <mergeCell ref="J63:Q63"/>
     <mergeCell ref="Y1:AF1"/>
-    <mergeCell ref="Y15:AF15"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:F40"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="J39:Q39"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:F17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="J15:Q15"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:F54"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="Y19:AF19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
measured the MI and c-p values (strategy) and made some plots - still need refininf
</commit_message>
<xml_diff>
--- a/Stats_Results.xlsx
+++ b/Stats_Results.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SSD_1Tb_PF/Work/torrey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C442B64E-1FF0-B344-98D6-B774EA1EA840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F7E05B-A9F2-4B46-A177-C2BA193A6F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{427BFFD6-8046-594F-BD1A-82F8D9FA486D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{427BFFD6-8046-594F-BD1A-82F8D9FA486D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Genus_Family_Ab" sheetId="1" r:id="rId1"/>
+    <sheet name="FeedingType" sheetId="3" r:id="rId2"/>
+    <sheet name="Diversity" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,8 +37,81 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={9AA3953B-86CB-344A-9ADE-DB32903EFA89}</author>
+    <author>tc={5E5E9703-487E-4B40-886B-6447147F87DE}</author>
+    <author>tc={88624626-B3D0-6C46-A8A8-FA5ACEC4AC30}</author>
+    <author>tc={956FEA81-D22D-A346-82AE-A7BD99CE9086}</author>
+    <author>tc={A9DD4C93-847F-3D46-A203-DAD14E39AF5D}</author>
+    <author>tc={7BD080FD-696D-7943-9A7B-BBDD089007AE}</author>
+    <author>tc={99BE7E7E-7A7E-AD42-8D8C-8F7F602EB135}</author>
+  </authors>
+  <commentList>
+    <comment ref="E26" authorId="0" shapeId="0" xr:uid="{9AA3953B-86CB-344A-9ADE-DB32903EFA89}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    IS_01 differs significantly from BB_01 and FPS_01 and IS_02</t>
+      </text>
+    </comment>
+    <comment ref="H26" authorId="1" shapeId="0" xr:uid="{5E5E9703-487E-4B40-886B-6447147F87DE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    IS_01 x IS_02 / IS_01 x FPS_01</t>
+      </text>
+    </comment>
+    <comment ref="E27" authorId="2" shapeId="0" xr:uid="{88624626-B3D0-6C46-A8A8-FA5ACEC4AC30}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not that significantt but FPS differ from Impacted</t>
+      </text>
+    </comment>
+    <comment ref="H27" authorId="3" shapeId="0" xr:uid="{956FEA81-D22D-A346-82AE-A7BD99CE9086}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Ns pairwise</t>
+      </text>
+    </comment>
+    <comment ref="E28" authorId="4" shapeId="0" xr:uid="{A9DD4C93-847F-3D46-A203-DAD14E39AF5D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    IS_01 differs significantly with all the others</t>
+      </text>
+    </comment>
+    <comment ref="F28" authorId="5" shapeId="0" xr:uid="{7BD080FD-696D-7943-9A7B-BBDD089007AE}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Only IS_01 with BB_
+02 </t>
+      </text>
+    </comment>
+    <comment ref="H28" authorId="6" shapeId="0" xr:uid="{99BE7E7E-7A7E-AD42-8D8C-8F7F602EB135}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    IS_01 is highly significantly different from all the others in terms of expected family diversity</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="139">
   <si>
     <t>Df</t>
   </si>
@@ -357,13 +432,109 @@
   </si>
   <si>
     <t>0.041</t>
+  </si>
+  <si>
+    <t>Habitat</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>ET_50</t>
+  </si>
+  <si>
+    <t>Bivalve beds</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>BB_01</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>FPS_01</t>
+  </si>
+  <si>
+    <t>IS_01</t>
+  </si>
+  <si>
+    <t>BB_02</t>
+  </si>
+  <si>
+    <t>IS_02</t>
+  </si>
+  <si>
+    <t>Station</t>
+  </si>
+  <si>
+    <t>Replicate</t>
+  </si>
+  <si>
+    <t>Genus diversity</t>
+  </si>
+  <si>
+    <t>Family diversity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One-way permanova </t>
+  </si>
+  <si>
+    <t>ns</t>
+  </si>
+  <si>
+    <t>Euclidean distance</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Genus</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>* .</t>
+  </si>
+  <si>
+    <t>Factors</t>
+  </si>
+  <si>
+    <t>Trophic guils</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               Df SumsOfSqs MeanSqs F.Model      R2 Pr(&gt;F)   </t>
+  </si>
+  <si>
+    <t>FT_w.1$Habitat  2    4266.4 2133.22  3.5368 0.37086 0.0069 **</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residuals      12    7237.8  603.15         0.62914          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total          14   11504.3                 1.00000          </t>
+  </si>
+  <si>
+    <t>Bivalve beds is significantly different from Impacted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -441,8 +612,14 @@
       <name val="Lucida Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,8 +686,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -518,11 +701,128 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -548,9 +848,12 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -558,12 +861,71 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,6 +941,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Francesca Pasotti" id="{21A1E381-EDB9-DD45-B5AF-6C8DA8D27530}" userId="76b8ee91e3e87ea5" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -896,12 +1264,39 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E26" dT="2025-03-25T10:52:08.72" personId="{21A1E381-EDB9-DD45-B5AF-6C8DA8D27530}" id="{9AA3953B-86CB-344A-9ADE-DB32903EFA89}">
+    <text>IS_01 differs significantly from BB_01 and FPS_01 and IS_02</text>
+  </threadedComment>
+  <threadedComment ref="H26" dT="2025-03-25T11:03:59.60" personId="{21A1E381-EDB9-DD45-B5AF-6C8DA8D27530}" id="{5E5E9703-487E-4B40-886B-6447147F87DE}">
+    <text>IS_01 x IS_02 / IS_01 x FPS_01</text>
+  </threadedComment>
+  <threadedComment ref="E27" dT="2025-03-25T10:53:59.35" personId="{21A1E381-EDB9-DD45-B5AF-6C8DA8D27530}" id="{88624626-B3D0-6C46-A8A8-FA5ACEC4AC30}">
+    <text>Not that significantt but FPS differ from Impacted</text>
+  </threadedComment>
+  <threadedComment ref="H27" dT="2025-03-25T10:57:02.10" personId="{21A1E381-EDB9-DD45-B5AF-6C8DA8D27530}" id="{956FEA81-D22D-A346-82AE-A7BD99CE9086}">
+    <text>Ns pairwise</text>
+  </threadedComment>
+  <threadedComment ref="E28" dT="2025-03-25T10:52:29.69" personId="{21A1E381-EDB9-DD45-B5AF-6C8DA8D27530}" id="{A9DD4C93-847F-3D46-A203-DAD14E39AF5D}">
+    <text>IS_01 differs significantly with all the others</text>
+  </threadedComment>
+  <threadedComment ref="F28" dT="2025-03-25T10:54:49.77" personId="{21A1E381-EDB9-DD45-B5AF-6C8DA8D27530}" id="{7BD080FD-696D-7943-9A7B-BBDD089007AE}">
+    <text xml:space="preserve">Only IS_01 with BB_
+02 </text>
+  </threadedComment>
+  <threadedComment ref="H28" dT="2025-03-25T10:56:40.95" personId="{21A1E381-EDB9-DD45-B5AF-6C8DA8D27530}" id="{99BE7E7E-7A7E-AD42-8D8C-8F7F602EB135}">
+    <text>IS_01 is highly significantly different from all the others in terms of expected family diversity</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EA06066-730F-AC47-8C37-A79A1AD98C17}">
   <dimension ref="A1:AF79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="137" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="137" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82:K92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -911,44 +1306,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="25" customHeight="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="J1" s="23" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="J1" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="Y1" s="23" t="s">
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="Y1" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="23"/>
-      <c r="AE1" s="23"/>
-      <c r="AF1" s="23"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
     </row>
     <row r="2" spans="1:32" ht="20">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
       <c r="J2" s="6" t="s">
         <v>12</v>
       </c>
@@ -1120,25 +1515,25 @@
       </c>
     </row>
     <row r="12" spans="1:32" ht="20">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="23" t="s">
         <v>90</v>
       </c>
       <c r="J12" s="6" t="s">
@@ -1149,25 +1544,25 @@
       <c r="P12" s="10"/>
     </row>
     <row r="13" spans="1:32" ht="20">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="G13" s="24" t="s">
         <v>86</v>
       </c>
       <c r="J13" s="6" t="s">
@@ -1178,25 +1573,25 @@
       <c r="N13" s="10"/>
     </row>
     <row r="14" spans="1:32" ht="20">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="26">
         <v>2411</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="25">
         <v>1</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="25">
         <v>7</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="27" t="s">
         <v>102</v>
       </c>
       <c r="J14" s="6"/>
@@ -1205,25 +1600,25 @@
       <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:32" ht="20">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="26">
         <v>3145</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="25">
         <v>1</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="25">
         <v>10</v>
       </c>
-      <c r="G15" s="32" t="s">
+      <c r="G15" s="28" t="s">
         <v>104</v>
       </c>
       <c r="J15" s="6"/>
@@ -1232,25 +1627,25 @@
       <c r="N15" s="10"/>
     </row>
     <row r="16" spans="1:32" ht="20">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="26">
         <v>2531</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="25">
         <v>1</v>
       </c>
-      <c r="F16" s="29">
+      <c r="F16" s="25">
         <v>7</v>
       </c>
-      <c r="G16" s="32" t="s">
+      <c r="G16" s="28" t="s">
         <v>106</v>
       </c>
       <c r="J16" s="6"/>
@@ -1265,64 +1660,64 @@
       <c r="N17" s="10"/>
     </row>
     <row r="19" spans="1:32" ht="22">
-      <c r="J19" s="23" t="s">
+      <c r="J19" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="Y19" s="23" t="s">
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="32"/>
+      <c r="Y19" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="Z19" s="23"/>
-      <c r="AA19" s="23"/>
-      <c r="AB19" s="23"/>
-      <c r="AC19" s="23"/>
-      <c r="AD19" s="23"/>
-      <c r="AE19" s="23"/>
-      <c r="AF19" s="23"/>
+      <c r="Z19" s="32"/>
+      <c r="AA19" s="32"/>
+      <c r="AB19" s="32"/>
+      <c r="AC19" s="32"/>
+      <c r="AD19" s="32"/>
+      <c r="AE19" s="32"/>
+      <c r="AF19" s="32"/>
     </row>
     <row r="20" spans="1:32" ht="20">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
       <c r="J20" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:32" ht="20">
-      <c r="A21" s="24"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
       <c r="J21" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:32" ht="20">
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D22" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="31" t="s">
         <v>40</v>
       </c>
       <c r="J22" s="6" t="s">
@@ -1339,10 +1734,10 @@
       <c r="A23" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
       <c r="J23" s="6" t="s">
         <v>43</v>
       </c>
@@ -1487,45 +1882,45 @@
     <row r="36" spans="1:29" s="14" customFormat="1"/>
     <row r="37" spans="1:29" s="14" customFormat="1"/>
     <row r="43" spans="1:29" ht="22">
-      <c r="A43" s="24" t="s">
+      <c r="A43" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B43" s="25" t="s">
+      <c r="B43" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
       <c r="G43" s="5"/>
-      <c r="J43" s="23" t="s">
+      <c r="J43" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="K43" s="23"/>
-      <c r="L43" s="23"/>
-      <c r="M43" s="23"/>
-      <c r="N43" s="23"/>
-      <c r="O43" s="23"/>
-      <c r="P43" s="23"/>
-      <c r="Q43" s="23"/>
-      <c r="V43" s="23" t="s">
+      <c r="K43" s="32"/>
+      <c r="L43" s="32"/>
+      <c r="M43" s="32"/>
+      <c r="N43" s="32"/>
+      <c r="O43" s="32"/>
+      <c r="P43" s="32"/>
+      <c r="Q43" s="32"/>
+      <c r="V43" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="W43" s="23"/>
-      <c r="X43" s="23"/>
-      <c r="Y43" s="23"/>
-      <c r="Z43" s="23"/>
-      <c r="AA43" s="23"/>
-      <c r="AB43" s="23"/>
-      <c r="AC43" s="23"/>
+      <c r="W43" s="32"/>
+      <c r="X43" s="32"/>
+      <c r="Y43" s="32"/>
+      <c r="Z43" s="32"/>
+      <c r="AA43" s="32"/>
+      <c r="AB43" s="32"/>
+      <c r="AC43" s="32"/>
     </row>
     <row r="44" spans="1:29" ht="22">
-      <c r="A44" s="24"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
+      <c r="A44" s="29"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
       <c r="G44" s="5"/>
       <c r="J44" s="6" t="s">
         <v>12</v>
@@ -1537,16 +1932,16 @@
       <c r="O44" s="7"/>
     </row>
     <row r="45" spans="1:29" ht="22">
-      <c r="B45" s="26" t="s">
+      <c r="B45" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="26" t="s">
+      <c r="C45" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="26" t="s">
+      <c r="D45" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E45" s="26" t="s">
+      <c r="E45" s="31" t="s">
         <v>40</v>
       </c>
       <c r="J45" s="6" t="s">
@@ -1565,10 +1960,10 @@
       <c r="A46" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
       <c r="G46" s="1"/>
       <c r="J46" s="6" t="s">
         <v>50</v>
@@ -1736,25 +2131,25 @@
       </c>
     </row>
     <row r="56" spans="1:29" ht="20">
-      <c r="A56" s="27" t="s">
+      <c r="A56" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B56" s="27" t="s">
+      <c r="B56" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C56" s="27" t="s">
+      <c r="C56" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D56" s="27" t="s">
+      <c r="D56" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="E56" s="27" t="s">
+      <c r="E56" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="F56" s="27" t="s">
+      <c r="F56" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="G56" s="27" t="s">
+      <c r="G56" s="23" t="s">
         <v>90</v>
       </c>
       <c r="J56" s="6"/>
@@ -1762,25 +2157,25 @@
       <c r="N56" s="10"/>
     </row>
     <row r="57" spans="1:29" ht="20">
-      <c r="A57" s="28" t="s">
+      <c r="A57" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="28" t="s">
+      <c r="B57" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C57" s="28" t="s">
+      <c r="C57" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="D57" s="28" t="s">
+      <c r="D57" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="E57" s="28" t="s">
+      <c r="E57" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="F57" s="28" t="s">
+      <c r="F57" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="G57" s="28" t="s">
+      <c r="G57" s="24" t="s">
         <v>86</v>
       </c>
       <c r="J57" s="6"/>
@@ -1788,25 +2183,25 @@
       <c r="N57" s="10"/>
     </row>
     <row r="58" spans="1:29" ht="20">
-      <c r="A58" s="29" t="s">
+      <c r="A58" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="B58" s="29" t="s">
+      <c r="B58" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="C58" s="29" t="s">
+      <c r="C58" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="D58" s="30">
+      <c r="D58" s="26">
         <v>1519</v>
       </c>
-      <c r="E58" s="29">
+      <c r="E58" s="25">
         <v>1</v>
       </c>
-      <c r="F58" s="29">
+      <c r="F58" s="25">
         <v>7</v>
       </c>
-      <c r="G58" s="29" t="s">
+      <c r="G58" s="25" t="s">
         <v>94</v>
       </c>
       <c r="J58" s="6"/>
@@ -1814,25 +2209,25 @@
       <c r="N58" s="10"/>
     </row>
     <row r="59" spans="1:29" ht="20">
-      <c r="A59" s="29" t="s">
+      <c r="A59" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="B59" s="29" t="s">
+      <c r="B59" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="C59" s="29" t="s">
+      <c r="C59" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="D59" s="30">
+      <c r="D59" s="26">
         <v>2526</v>
       </c>
-      <c r="E59" s="29">
+      <c r="E59" s="25">
         <v>1</v>
       </c>
-      <c r="F59" s="29">
+      <c r="F59" s="25">
         <v>10</v>
       </c>
-      <c r="G59" s="31" t="s">
+      <c r="G59" s="27" t="s">
         <v>97</v>
       </c>
       <c r="J59" s="6"/>
@@ -1840,25 +2235,25 @@
       <c r="N59" s="10"/>
     </row>
     <row r="60" spans="1:29" ht="20">
-      <c r="A60" s="29" t="s">
+      <c r="A60" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="B60" s="29" t="s">
+      <c r="B60" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="C60" s="29" t="s">
+      <c r="C60" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="D60" s="30">
+      <c r="D60" s="26">
         <v>1576</v>
       </c>
-      <c r="E60" s="29">
+      <c r="E60" s="25">
         <v>1</v>
       </c>
-      <c r="F60" s="29">
+      <c r="F60" s="25">
         <v>7</v>
       </c>
-      <c r="G60" s="29" t="s">
+      <c r="G60" s="25" t="s">
         <v>99</v>
       </c>
       <c r="J60" s="6"/>
@@ -1872,44 +2267,44 @@
       <c r="J62" s="6"/>
     </row>
     <row r="63" spans="1:29" ht="22">
-      <c r="A63" s="24" t="s">
+      <c r="A63" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B63" s="25" t="s">
+      <c r="B63" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="25"/>
-      <c r="J63" s="23" t="s">
+      <c r="C63" s="30"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="30"/>
+      <c r="J63" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="K63" s="23"/>
-      <c r="L63" s="23"/>
-      <c r="M63" s="23"/>
-      <c r="N63" s="23"/>
-      <c r="O63" s="23"/>
-      <c r="P63" s="23"/>
-      <c r="Q63" s="23"/>
-      <c r="V63" s="23" t="s">
+      <c r="K63" s="32"/>
+      <c r="L63" s="32"/>
+      <c r="M63" s="32"/>
+      <c r="N63" s="32"/>
+      <c r="O63" s="32"/>
+      <c r="P63" s="32"/>
+      <c r="Q63" s="32"/>
+      <c r="V63" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="W63" s="23"/>
-      <c r="X63" s="23"/>
-      <c r="Y63" s="23"/>
-      <c r="Z63" s="23"/>
-      <c r="AA63" s="23"/>
-      <c r="AB63" s="23"/>
-      <c r="AC63" s="23"/>
+      <c r="W63" s="32"/>
+      <c r="X63" s="32"/>
+      <c r="Y63" s="32"/>
+      <c r="Z63" s="32"/>
+      <c r="AA63" s="32"/>
+      <c r="AB63" s="32"/>
+      <c r="AC63" s="32"/>
     </row>
     <row r="64" spans="1:29">
-      <c r="A64" s="24"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
+      <c r="A64" s="29"/>
+      <c r="B64" s="30"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="30"/>
     </row>
     <row r="65" spans="1:27" ht="20">
       <c r="J65" s="6" t="s">
@@ -1917,16 +2312,16 @@
       </c>
     </row>
     <row r="66" spans="1:27" ht="20">
-      <c r="B66" s="26" t="s">
+      <c r="B66" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C66" s="26" t="s">
+      <c r="C66" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D66" s="26" t="s">
+      <c r="D66" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E66" s="26" t="s">
+      <c r="E66" s="31" t="s">
         <v>40</v>
       </c>
       <c r="J66" s="6" t="s">
@@ -1940,10 +2335,10 @@
       <c r="A67" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B67" s="26"/>
-      <c r="C67" s="26"/>
-      <c r="D67" s="26"/>
-      <c r="E67" s="26"/>
+      <c r="B67" s="31"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="31"/>
       <c r="J67" s="6" t="s">
         <v>57</v>
       </c>
@@ -2100,17 +2495,11 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:F64"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="V43:AC43"/>
+    <mergeCell ref="V63:AC63"/>
+    <mergeCell ref="J63:Q63"/>
+    <mergeCell ref="Y1:AF1"/>
+    <mergeCell ref="Y19:AF19"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:F44"/>
@@ -2123,12 +2512,828 @@
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="E22:E23"/>
     <mergeCell ref="J19:Q19"/>
-    <mergeCell ref="V43:AC43"/>
-    <mergeCell ref="V63:AC63"/>
-    <mergeCell ref="J63:Q63"/>
-    <mergeCell ref="Y1:AF1"/>
-    <mergeCell ref="Y19:AF19"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:F64"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB2C59D7-48B3-0540-A9EB-46E169E32640}">
+  <dimension ref="A2:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="2" spans="1:10">
+      <c r="A2" s="57" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="20">
+      <c r="A4" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="20">
+      <c r="A5" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="20">
+      <c r="A6" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" ht="20">
+      <c r="A7" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="20">
+      <c r="A8" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="B9" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DEEE54A-9137-FF49-9FCE-36BA2819E35A}">
+  <dimension ref="B2:L41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12">
+      <c r="D2" s="33"/>
+    </row>
+    <row r="3" spans="2:12">
+      <c r="B3" s="58"/>
+      <c r="C3" s="59" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="60"/>
+      <c r="E3" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="42"/>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="J4" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="K4" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="L4" s="36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="44">
+        <v>24</v>
+      </c>
+      <c r="F5" s="44">
+        <v>2.5630829999999998</v>
+      </c>
+      <c r="G5" s="44">
+        <v>0.80649459999999995</v>
+      </c>
+      <c r="H5" s="44">
+        <v>15.92238</v>
+      </c>
+      <c r="I5" s="44">
+        <v>14</v>
+      </c>
+      <c r="J5" s="44">
+        <v>1.976156</v>
+      </c>
+      <c r="K5" s="44">
+        <v>0.74881140000000002</v>
+      </c>
+      <c r="L5" s="45">
+        <v>10.320410000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="B6" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="47">
+        <v>20</v>
+      </c>
+      <c r="F6" s="47">
+        <v>2.5433110000000001</v>
+      </c>
+      <c r="G6" s="47">
+        <v>0.84897789999999995</v>
+      </c>
+      <c r="H6" s="47">
+        <v>15.8589</v>
+      </c>
+      <c r="I6" s="47">
+        <v>15</v>
+      </c>
+      <c r="J6" s="47">
+        <v>2.2482989999999998</v>
+      </c>
+      <c r="K6" s="47">
+        <v>0.83022790000000002</v>
+      </c>
+      <c r="L6" s="48">
+        <v>12.32916</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="47">
+        <v>25</v>
+      </c>
+      <c r="F7" s="47">
+        <v>2.742969</v>
+      </c>
+      <c r="G7" s="47">
+        <v>0.8521514</v>
+      </c>
+      <c r="H7" s="47">
+        <v>17.38307</v>
+      </c>
+      <c r="I7" s="47">
+        <v>14</v>
+      </c>
+      <c r="J7" s="47">
+        <v>2.2174100000000001</v>
+      </c>
+      <c r="K7" s="47">
+        <v>0.84022819999999998</v>
+      </c>
+      <c r="L7" s="48">
+        <v>10.936909999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="B8" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" s="47">
+        <v>25</v>
+      </c>
+      <c r="F8" s="47">
+        <v>2.743474</v>
+      </c>
+      <c r="G8" s="47">
+        <v>0.85230799999999995</v>
+      </c>
+      <c r="H8" s="47">
+        <v>17.159140000000001</v>
+      </c>
+      <c r="I8" s="47">
+        <v>14</v>
+      </c>
+      <c r="J8" s="47">
+        <v>2.2181549999999999</v>
+      </c>
+      <c r="K8" s="47">
+        <v>0.84051039999999999</v>
+      </c>
+      <c r="L8" s="48">
+        <v>10.81161</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="B9" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" s="47">
+        <v>22</v>
+      </c>
+      <c r="F9" s="47">
+        <v>2.3038099999999999</v>
+      </c>
+      <c r="G9" s="47">
+        <v>0.74531820000000004</v>
+      </c>
+      <c r="H9" s="47">
+        <v>14.94482</v>
+      </c>
+      <c r="I9" s="47">
+        <v>14</v>
+      </c>
+      <c r="J9" s="47">
+        <v>1.9278040000000001</v>
+      </c>
+      <c r="K9" s="47">
+        <v>0.73048950000000001</v>
+      </c>
+      <c r="L9" s="48">
+        <v>10.37454</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
+      <c r="B10" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="47">
+        <v>21</v>
+      </c>
+      <c r="F10" s="47">
+        <v>2.3700559999999999</v>
+      </c>
+      <c r="G10" s="47">
+        <v>0.77846559999999998</v>
+      </c>
+      <c r="H10" s="47">
+        <v>14.51661</v>
+      </c>
+      <c r="I10" s="47">
+        <v>14</v>
+      </c>
+      <c r="J10" s="47">
+        <v>2.1193740000000001</v>
+      </c>
+      <c r="K10" s="47">
+        <v>0.80308000000000002</v>
+      </c>
+      <c r="L10" s="48">
+        <v>10.995039999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12">
+      <c r="B11" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" s="47">
+        <v>37</v>
+      </c>
+      <c r="F11" s="47">
+        <v>3.1487400000000001</v>
+      </c>
+      <c r="G11" s="47">
+        <v>0.87200540000000004</v>
+      </c>
+      <c r="H11" s="47">
+        <v>24.770330000000001</v>
+      </c>
+      <c r="I11" s="47">
+        <v>24</v>
+      </c>
+      <c r="J11" s="47">
+        <v>2.6607810000000001</v>
+      </c>
+      <c r="K11" s="47">
+        <v>0.83723590000000003</v>
+      </c>
+      <c r="L11" s="48">
+        <v>17.162199999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12">
+      <c r="B12" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" s="47">
+        <v>33</v>
+      </c>
+      <c r="F12" s="47">
+        <v>2.8923040000000002</v>
+      </c>
+      <c r="G12" s="47">
+        <v>0.82719799999999999</v>
+      </c>
+      <c r="H12" s="47">
+        <v>20.73875</v>
+      </c>
+      <c r="I12" s="47">
+        <v>20</v>
+      </c>
+      <c r="J12" s="47">
+        <v>2.4691960000000002</v>
+      </c>
+      <c r="K12" s="47">
+        <v>0.82423800000000003</v>
+      </c>
+      <c r="L12" s="48">
+        <v>15.086639999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
+      <c r="B13" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="E13" s="47">
+        <v>30</v>
+      </c>
+      <c r="F13" s="47">
+        <v>2.7755139999999998</v>
+      </c>
+      <c r="G13" s="47">
+        <v>0.8160404</v>
+      </c>
+      <c r="H13" s="47">
+        <v>19.382100000000001</v>
+      </c>
+      <c r="I13" s="47">
+        <v>22</v>
+      </c>
+      <c r="J13" s="47">
+        <v>2.5530780000000002</v>
+      </c>
+      <c r="K13" s="47">
+        <v>0.82596009999999997</v>
+      </c>
+      <c r="L13" s="48">
+        <v>15.716189999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12">
+      <c r="B14" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="47">
+        <v>29</v>
+      </c>
+      <c r="F14" s="47">
+        <v>2.8190230000000001</v>
+      </c>
+      <c r="G14" s="47">
+        <v>0.83717710000000001</v>
+      </c>
+      <c r="H14" s="47">
+        <v>19.918579999999999</v>
+      </c>
+      <c r="I14" s="47">
+        <v>19</v>
+      </c>
+      <c r="J14" s="47">
+        <v>2.182884</v>
+      </c>
+      <c r="K14" s="47">
+        <v>0.74135819999999997</v>
+      </c>
+      <c r="L14" s="48">
+        <v>13.10416</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" s="47">
+        <v>23</v>
+      </c>
+      <c r="F15" s="47">
+        <v>2.4596360000000002</v>
+      </c>
+      <c r="G15" s="47">
+        <v>0.78444910000000001</v>
+      </c>
+      <c r="H15" s="47">
+        <v>16.041620000000002</v>
+      </c>
+      <c r="I15" s="47">
+        <v>14</v>
+      </c>
+      <c r="J15" s="47">
+        <v>1.9408160000000001</v>
+      </c>
+      <c r="K15" s="47">
+        <v>0.73542019999999997</v>
+      </c>
+      <c r="L15" s="48">
+        <v>10.417809999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12">
+      <c r="B16" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="47">
+        <v>30</v>
+      </c>
+      <c r="F16" s="47">
+        <v>2.5257239999999999</v>
+      </c>
+      <c r="G16" s="47">
+        <v>0.7425986</v>
+      </c>
+      <c r="H16" s="47">
+        <v>18.458880000000001</v>
+      </c>
+      <c r="I16" s="47">
+        <v>16</v>
+      </c>
+      <c r="J16" s="47">
+        <v>1.674607</v>
+      </c>
+      <c r="K16" s="47">
+        <v>0.60398689999999999</v>
+      </c>
+      <c r="L16" s="48">
+        <v>10.623139999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
+      <c r="B17" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>119</v>
+      </c>
+      <c r="E17" s="47">
+        <v>24</v>
+      </c>
+      <c r="F17" s="47">
+        <v>2.5410249999999999</v>
+      </c>
+      <c r="G17" s="47">
+        <v>0.79955379999999998</v>
+      </c>
+      <c r="H17" s="47">
+        <v>16.606909999999999</v>
+      </c>
+      <c r="I17" s="47">
+        <v>18</v>
+      </c>
+      <c r="J17" s="47">
+        <v>2.2781769999999999</v>
+      </c>
+      <c r="K17" s="47">
+        <v>0.78819499999999998</v>
+      </c>
+      <c r="L17" s="48">
+        <v>13.11661</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="B18" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>119</v>
+      </c>
+      <c r="E18" s="47">
+        <v>26</v>
+      </c>
+      <c r="F18" s="47">
+        <v>2.4506019999999999</v>
+      </c>
+      <c r="G18" s="47">
+        <v>0.75215759999999998</v>
+      </c>
+      <c r="H18" s="47">
+        <v>16.817019999999999</v>
+      </c>
+      <c r="I18" s="47">
+        <v>17</v>
+      </c>
+      <c r="J18" s="47">
+        <v>2.0398909999999999</v>
+      </c>
+      <c r="K18" s="47">
+        <v>0.71999199999999997</v>
+      </c>
+      <c r="L18" s="48">
+        <v>11.79692</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12">
+      <c r="B19" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="E19" s="50">
+        <v>21</v>
+      </c>
+      <c r="F19" s="50">
+        <v>2.0673270000000001</v>
+      </c>
+      <c r="G19" s="50">
+        <v>0.67903159999999996</v>
+      </c>
+      <c r="H19" s="50">
+        <v>13.81142</v>
+      </c>
+      <c r="I19" s="50">
+        <v>14</v>
+      </c>
+      <c r="J19" s="50">
+        <v>1.854733</v>
+      </c>
+      <c r="K19" s="50">
+        <v>0.70280129999999996</v>
+      </c>
+      <c r="L19" s="51">
+        <v>10.402200000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12">
+      <c r="E23" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="G23" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="I23" s="53"/>
+    </row>
+    <row r="24" spans="2:12">
+      <c r="E24" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24" s="55" t="s">
+        <v>110</v>
+      </c>
+      <c r="H24" s="56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12">
+      <c r="C25" s="57" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="F25" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="G25" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="H25" s="57" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12">
+      <c r="C26" s="57" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="E26" s="57" t="s">
+        <v>129</v>
+      </c>
+      <c r="F26" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="G26" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="H26" s="57" t="s">
+        <v>129</v>
+      </c>
+      <c r="I26" s="53"/>
+    </row>
+    <row r="27" spans="2:12">
+      <c r="C27" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12">
+      <c r="C28" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="2:12">
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="2:12">
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="2:12">
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="4:4">
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="4:4">
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="4:4">
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="4:4">
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="4:4">
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="4:4">
+      <c r="D41" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="I3:L3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>